<commit_message>
Modification ergonomie écran action Chantier suppression process et composant, prix de reprise facultatif (SPCPRF) : structures de base de données, écrans de saisie prix reprise et répartitions, état mensuel collectivité HCS, état trimestriel collectivite CS, état menusel des réceptions.
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
+++ b/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Repos\Valorplast\eValorplastWebApp\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BAABE5-DA1D-4D93-9088-0074877D2FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F491E-3978-4E7A-A29F-1B12E2AB5BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12648" yWindow="4200" windowWidth="23364" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16392" yWindow="3864" windowWidth="25884" windowHeight="19248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etat" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>RS</t>
   </si>
@@ -50,24 +50,10 @@
   </si>
   <si>
     <t>EMBALLAGES PLASTIQUE</t>
-  </si>
-  <si>
-    <t>PROCESS</t>
-  </si>
-  <si>
-    <t>COMPOSANT</t>
-  </si>
-  <si>
-    <t>COUT DE SURTRI 
-(-€HT/t)</t>
   </si>
   <si>
     <t>PRIX DE REPRISE 
 (€HT/t)</t>
-  </si>
-  <si>
-    <t>COUT DE TRANSPORT 
-(-€HT/t)</t>
   </si>
   <si>
     <t>POIDS 
@@ -134,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -146,32 +132,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -297,24 +257,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,21 +298,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,7 +651,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:K46"/>
+  <dimension ref="A4:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -707,7 +663,8 @@
     <col min="4" max="4" width="29" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.8984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.09765625" style="1" customWidth="1"/>
-    <col min="7" max="11" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="17.796875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="10.59765625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -730,49 +687,49 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="7"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
+      <c r="D9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
+      <c r="D10" s="6"/>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="7"/>
+      <c r="D11" s="6"/>
       <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="11" t="s">
-        <v>17</v>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="12" t="s">
-        <v>16</v>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
@@ -781,19 +738,19 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -801,411 +758,445 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="21"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="21"/>
+      <c r="D21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
       <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
       <c r="K32" s="4"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
       <c r="K33" s="4"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
       <c r="K35" s="4"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
       <c r="K36" s="4"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
       <c r="K37" s="4"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
       <c r="K39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
       <c r="K40" s="4"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
+    <row r="42" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
       <c r="K42" s="4"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
       <c r="K43" s="4"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
       <c r="K44" s="4"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
       <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
       <c r="K46" s="4"/>
     </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A29:B29"/>
+  <mergeCells count="61">
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
     <mergeCell ref="C16:E17"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Chantier SPCPRF :  Remise en place des sous-totaux dans les états. Suppression des calculs de prix total dans les états (PU*Poids)
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
+++ b/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F491E-3978-4E7A-A29F-1B12E2AB5BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A211425-B765-4B39-B862-4E6287077CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16392" yWindow="3864" windowWidth="25884" windowHeight="19248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12636" yWindow="4464" windowWidth="25884" windowHeight="19248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etat" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>RS</t>
   </si>
@@ -67,10 +67,6 @@
   </si>
   <si>
     <t>Cet état vous sert de base pour établir la facture à Valorplast.</t>
-  </si>
-  <si>
-    <t>TOTAL 
-(€HT)</t>
   </si>
   <si>
     <t xml:space="preserve">pour </t>
@@ -651,7 +647,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:K50"/>
+  <dimension ref="A4:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,102 +659,100 @@
     <col min="4" max="4" width="29" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.8984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.09765625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="17.796875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="10.59765625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="1"/>
+    <col min="7" max="8" width="22.19921875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.59765625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:9" ht="21" x14ac:dyDescent="0.4">
       <c r="E4" s="3"/>
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="3:10" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="3:9" ht="21" x14ac:dyDescent="0.4">
       <c r="E5" s="3"/>
       <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D7" s="6"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D10" s="6"/>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" s="6"/>
       <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="17"/>
       <c r="G16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>6</v>
       </c>
@@ -775,13 +769,10 @@
       <c r="H21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -791,10 +782,9 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -804,10 +794,9 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -817,10 +806,9 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -830,10 +818,9 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -843,10 +830,9 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -856,10 +842,9 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -869,10 +854,9 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -882,10 +866,9 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -895,10 +878,9 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -908,10 +890,9 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -921,10 +902,9 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -934,10 +914,9 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -947,10 +926,9 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -960,10 +938,9 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -973,10 +950,9 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -986,10 +962,9 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -999,10 +974,9 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -1012,10 +986,9 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -1025,10 +998,9 @@
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -1038,19 +1010,18 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -1060,10 +1031,9 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -1073,10 +1043,9 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -1086,10 +1055,9 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -1099,10 +1067,9 @@
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -1110,7 +1077,7 @@
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>

</xml_diff>

<commit_message>
Sélection parmi les contacts BL actifs pour les nouvelles demandes d'enlèvement Totaux de type comptabilité pour les états mensuels HCS Affichages des parties CS ou HCS dans les répartition si des données existent MEP
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
+++ b/eVaSys.Server/Assets/Templates/EtatMensuelCollectiviteHCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F4408A-143A-4021-ACB5-52FE604E8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F10EF4B-BA95-4449-9E1C-C446CBC23BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6636" yWindow="4272" windowWidth="20736" windowHeight="18912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="2460" windowWidth="27732" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etat" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>RS</t>
   </si>
@@ -70,6 +70,10 @@
   </si>
   <si>
     <t xml:space="preserve">Paris le </t>
+  </si>
+  <si>
+    <t>TOTAL 
+(€HT/t)</t>
   </si>
 </sst>
 </file>
@@ -266,10 +270,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,9 +296,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,7 +648,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:J50"/>
+  <dimension ref="A4:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -656,28 +660,30 @@
     <col min="4" max="4" width="29" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.8984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.09765625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="22.19921875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.59765625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11" style="1"/>
+    <col min="7" max="9" width="15.3984375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="10.59765625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:10" ht="21" x14ac:dyDescent="0.4">
       <c r="E4" s="3"/>
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="3:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="3:10" ht="21" x14ac:dyDescent="0.4">
       <c r="E5" s="3"/>
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
@@ -685,424 +691,481 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D7" s="6"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D10" s="6"/>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D11" s="6"/>
       <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D13" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+    <row r="20" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="11"/>
+      <c r="I21" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A47:C47"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A50:C50"/>
@@ -1119,43 +1182,14 @@
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>